<commit_message>
testing equation display fix on documentation
</commit_message>
<xml_diff>
--- a/Pintle/Pintle_V3_Testing raw data/flow rate graph.xlsx
+++ b/Pintle/Pintle_V3_Testing raw data/flow rate graph.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jntil\Documents\Git_Repos\liquid-engine-test-stand\Pintle\Pintle_V3_Testing raw data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{364D9B72-18FF-4155-980B-27D7DA984001}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A373CD2D-326F-4CC0-A852-C6F1899A15FF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5865" yWindow="105" windowWidth="13830" windowHeight="10590" xr2:uid="{1C337766-0B60-4982-99F7-C0C8567B4E66}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11640" xr2:uid="{1C337766-0B60-4982-99F7-C0C8567B4E66}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,6 +28,44 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+  <si>
+    <t>Annulus</t>
+  </si>
+  <si>
+    <t>Pintle</t>
+  </si>
+  <si>
+    <t>intercept</t>
+  </si>
+  <si>
+    <t>slope</t>
+  </si>
+  <si>
+    <t>gpm</t>
+  </si>
+  <si>
+    <t>psi</t>
+  </si>
+  <si>
+    <t>gpm to m^3</t>
+  </si>
+  <si>
+    <t>density</t>
+  </si>
+  <si>
+    <t>mdot</t>
+  </si>
+  <si>
+    <t>psi to kpa</t>
+  </si>
+  <si>
+    <t>pa</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -67,7 +105,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -75,6 +113,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -255,7 +294,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$C$4:$J$4</c:f>
+              <c:f>Sheet1!$D$4:$K$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -288,7 +327,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$7:$J$7</c:f>
+              <c:f>Sheet1!$D$7:$K$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -513,7 +552,580 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>run 1</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-5.6405323636221451E-2"/>
+                  <c:y val="-2.1178920999486324E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$31:$K$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1716666667</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.23499999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.28666666670000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.40666666670000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.45500000000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.52166666669999995</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.57999999999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$29:$K$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.75</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.25</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4B5E-452D-BD7D-F3D8A40DACE8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="481173992"/>
+        <c:axId val="481179896"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredScatterSeries>
+              <c15:ser>
+                <c:idx val="1"/>
+                <c:order val="1"/>
+                <c:tx>
+                  <c:v>run 2</c:v>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="25400" cap="rnd">
+                    <a:noFill/>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent2"/>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent2"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:trendline>
+                  <c:spPr>
+                    <a:ln w="19050" cap="rnd">
+                      <a:solidFill>
+                        <a:schemeClr val="accent2"/>
+                      </a:solidFill>
+                      <a:prstDash val="sysDot"/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                  <c:trendlineType val="linear"/>
+                  <c:dispRSqr val="0"/>
+                  <c:dispEq val="0"/>
+                </c:trendline>
+                <c:xVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$C$32:$K$32</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="9"/>
+                      <c:pt idx="0">
+                        <c:v>0.1</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>0.15666666670000001</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>0.2033333333</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>0.255</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>0.30499999999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>0.35499999999999998</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>0.4</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>0.45500000000000002</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>0.51666666670000005</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:xVal>
+                <c:yVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$C$29:$K$29</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="9"/>
+                      <c:pt idx="0">
+                        <c:v>0.5</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>0.75</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>1.25</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>1.5</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>1.75</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>2.25</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>2.5</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:yVal>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000001-4B5E-452D-BD7D-F3D8A40DACE8}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredScatterSeries>
+          </c:ext>
+        </c:extLst>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="481173992"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="481179896"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="481179896"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="481173992"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1069,6 +1681,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1079,7 +2207,7 @@
       <xdr:rowOff>4762</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>95250</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
@@ -1102,6 +2230,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>9524</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C6C53533-18D4-40FF-8FDB-5CA2DC184F00}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1407,150 +2571,572 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72825900-4A0F-44B2-92CC-59237FF73251}">
-  <dimension ref="C4:O7"/>
+  <dimension ref="A4:R42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView tabSelected="1" topLeftCell="K21" workbookViewId="0">
+      <selection activeCell="Q40" sqref="Q40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="15" width="6.28515625" customWidth="1"/>
+    <col min="4" max="15" width="6.28515625" customWidth="1"/>
+    <col min="16" max="16" width="9.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C4" s="1">
+    <row r="4" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="D4" s="1">
         <v>0.5</v>
       </c>
-      <c r="D4" s="1">
+      <c r="E4" s="1">
         <v>0.75</v>
       </c>
-      <c r="E4" s="1">
+      <c r="F4" s="1">
         <v>1</v>
       </c>
-      <c r="F4" s="1">
+      <c r="G4" s="1">
         <v>1.25</v>
       </c>
-      <c r="G4" s="1">
+      <c r="H4" s="1">
         <v>1.5</v>
       </c>
-      <c r="H4" s="1">
+      <c r="I4" s="1">
         <v>1.75</v>
       </c>
-      <c r="I4" s="1">
+      <c r="J4" s="1">
         <v>2</v>
       </c>
-      <c r="J4" s="1">
+      <c r="K4" s="1">
         <v>2.25</v>
       </c>
-      <c r="K4" s="1">
+      <c r="L4" s="1">
         <v>2.5</v>
       </c>
-      <c r="L4" s="1">
+      <c r="M4" s="1">
         <v>2.75</v>
       </c>
-      <c r="M4" s="1">
+      <c r="N4" s="1">
         <v>3</v>
       </c>
-      <c r="N4" s="1">
+      <c r="O4" s="1">
         <v>3.25</v>
       </c>
-      <c r="O4" s="1">
+      <c r="P4" s="1">
         <v>3.5</v>
       </c>
     </row>
-    <row r="5" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C5" s="2">
+    <row r="5" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="D5" s="2">
         <v>33</v>
       </c>
-      <c r="D5" s="2">
+      <c r="E5" s="2">
         <v>16</v>
       </c>
-      <c r="E5" s="2">
+      <c r="F5" s="2">
         <v>20</v>
       </c>
-      <c r="F5" s="2">
+      <c r="G5" s="2">
         <v>22</v>
       </c>
-      <c r="G5" s="2">
+      <c r="H5" s="2">
         <v>29</v>
       </c>
-      <c r="H5" s="2">
+      <c r="I5" s="2">
         <v>36</v>
       </c>
-      <c r="I5" s="2">
+      <c r="J5" s="2">
         <v>19</v>
       </c>
-      <c r="J5" s="2">
+      <c r="K5" s="2">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C6">
-        <f>C5</f>
+    <row r="6" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <f>D5</f>
         <v>33</v>
       </c>
-      <c r="D6">
-        <f>C5+D5</f>
+      <c r="E6">
+        <f>D5+E5</f>
         <v>49</v>
       </c>
-      <c r="E6">
-        <f>D6+E5</f>
+      <c r="F6">
+        <f t="shared" ref="F6:K6" si="0">E6+F5</f>
         <v>69</v>
       </c>
-      <c r="F6">
-        <f>E6+F5</f>
+      <c r="G6">
+        <f t="shared" si="0"/>
         <v>91</v>
       </c>
-      <c r="G6">
-        <f>F6+G5</f>
+      <c r="H6">
+        <f t="shared" si="0"/>
         <v>120</v>
       </c>
-      <c r="H6">
-        <f>G6+H5</f>
+      <c r="I6">
+        <f t="shared" si="0"/>
         <v>156</v>
       </c>
-      <c r="I6">
-        <f>H6+I5</f>
+      <c r="J6">
+        <f t="shared" si="0"/>
         <v>175</v>
       </c>
-      <c r="J6">
-        <f>I6+J5</f>
+      <c r="K6">
+        <f t="shared" si="0"/>
         <v>190</v>
       </c>
     </row>
-    <row r="7" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C7">
-        <f>C6/60</f>
+    <row r="7" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <f>D6/60</f>
         <v>0.55000000000000004</v>
       </c>
-      <c r="D7">
-        <f t="shared" ref="D7:J7" si="0">D6/60</f>
+      <c r="E7">
+        <f t="shared" ref="E7:K7" si="1">E6/60</f>
         <v>0.81666666666666665</v>
       </c>
-      <c r="E7">
-        <f t="shared" si="0"/>
+      <c r="F7">
+        <f t="shared" si="1"/>
         <v>1.1499999999999999</v>
       </c>
-      <c r="F7">
-        <f t="shared" si="0"/>
+      <c r="G7">
+        <f t="shared" si="1"/>
         <v>1.5166666666666666</v>
       </c>
-      <c r="G7">
-        <f t="shared" si="0"/>
+      <c r="H7">
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="H7">
-        <f t="shared" si="0"/>
+      <c r="I7">
+        <f t="shared" si="1"/>
         <v>2.6</v>
       </c>
-      <c r="I7">
-        <f t="shared" si="0"/>
+      <c r="J7">
+        <f t="shared" si="1"/>
         <v>2.9166666666666665</v>
       </c>
-      <c r="J7">
-        <f t="shared" si="0"/>
+      <c r="K7">
+        <f t="shared" si="1"/>
         <v>3.1666666666666665</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P23" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>7</v>
+      </c>
+      <c r="R23" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P24" s="3">
+        <v>6.3090199999999994E-5</v>
+      </c>
+      <c r="Q24">
+        <v>999.7</v>
+      </c>
+      <c r="R24">
+        <v>0.14503769999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C29">
+        <v>0.5</v>
+      </c>
+      <c r="D29">
+        <v>0.75</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29">
+        <v>1.25</v>
+      </c>
+      <c r="G29">
+        <v>1.5</v>
+      </c>
+      <c r="H29">
+        <v>1.75</v>
+      </c>
+      <c r="I29">
+        <v>2</v>
+      </c>
+      <c r="J29">
+        <v>2.25</v>
+      </c>
+      <c r="K29">
+        <v>2.5</v>
+      </c>
+      <c r="O29" t="s">
+        <v>4</v>
+      </c>
+      <c r="P29" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>5</v>
+      </c>
+      <c r="R29" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="N30" t="s">
+        <v>2</v>
+      </c>
+      <c r="O30" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>0</v>
+      </c>
+      <c r="B31">
+        <v>20</v>
+      </c>
+      <c r="C31">
+        <v>0.1</v>
+      </c>
+      <c r="D31">
+        <v>0.1716666667</v>
+      </c>
+      <c r="E31">
+        <v>0.23499999999999999</v>
+      </c>
+      <c r="F31">
+        <v>0.28666666670000002</v>
+      </c>
+      <c r="G31">
+        <v>0.35</v>
+      </c>
+      <c r="H31">
+        <v>0.40666666670000001</v>
+      </c>
+      <c r="I31">
+        <v>0.45500000000000002</v>
+      </c>
+      <c r="J31">
+        <v>0.52166666669999995</v>
+      </c>
+      <c r="K31">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="N31">
+        <f>INTERCEPT(C29:K29,C31:K31)</f>
+        <v>3.5000118685009962E-2</v>
+      </c>
+      <c r="O31">
+        <f>SLOPE($C$29:$K$29,C31:K31)</f>
+        <v>4.2440983684342379</v>
+      </c>
+      <c r="P31" s="3">
+        <f>O31*$P$24*$Q$24</f>
+        <v>0.26768068657972449</v>
+      </c>
+      <c r="Q31">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="R31">
+        <f>(Q31/$R$24)*1000</f>
+        <v>111005.62129708346</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B32">
+        <v>20</v>
+      </c>
+      <c r="C32">
+        <v>0.1</v>
+      </c>
+      <c r="D32">
+        <v>0.15666666670000001</v>
+      </c>
+      <c r="E32">
+        <v>0.2033333333</v>
+      </c>
+      <c r="F32">
+        <v>0.255</v>
+      </c>
+      <c r="G32">
+        <v>0.30499999999999999</v>
+      </c>
+      <c r="H32">
+        <v>0.35499999999999998</v>
+      </c>
+      <c r="I32">
+        <v>0.4</v>
+      </c>
+      <c r="J32">
+        <v>0.45500000000000002</v>
+      </c>
+      <c r="K32">
+        <v>0.51666666670000005</v>
+      </c>
+      <c r="N32">
+        <f>INTERCEPT(C29:K29,C32:K32)</f>
+        <v>2.9022282519461928E-3</v>
+      </c>
+      <c r="O32">
+        <f>SLOPE($C$29:$K$29,C32:K32)</f>
+        <v>4.9055388151343324</v>
+      </c>
+      <c r="P32" s="3">
+        <f>O32*$P$24*$Q$24</f>
+        <v>0.30939857752710165</v>
+      </c>
+      <c r="Q32">
+        <v>19.2</v>
+      </c>
+      <c r="R32">
+        <f>(Q32/$R$24)*1000</f>
+        <v>132379.37446608709</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <v>20</v>
+      </c>
+      <c r="C33">
+        <v>8.1666666669999999E-2</v>
+      </c>
+      <c r="D33">
+        <v>0.13</v>
+      </c>
+      <c r="E33">
+        <v>0.17833333330000001</v>
+      </c>
+      <c r="F33">
+        <v>0.23</v>
+      </c>
+      <c r="G33">
+        <v>0.29166666670000002</v>
+      </c>
+      <c r="H33">
+        <v>0.33666666670000001</v>
+      </c>
+      <c r="I33">
+        <v>0.39333333329999998</v>
+      </c>
+      <c r="J33">
+        <v>0.44333333330000002</v>
+      </c>
+      <c r="K33">
+        <v>0.49</v>
+      </c>
+      <c r="N33">
+        <f>INTERCEPT($C$29:$K$29,C33:K33)</f>
+        <v>0.12093163421712005</v>
+      </c>
+      <c r="O33">
+        <f>SLOPE($C$29:$K$29,C33:K33)</f>
+        <v>4.8200447736662211</v>
+      </c>
+      <c r="P33" s="3">
+        <f>O33*$P$24*$Q$24</f>
+        <v>0.30400635950292276</v>
+      </c>
+      <c r="Q33">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="R33">
+        <f>(Q33/$R$24)*1000</f>
+        <v>130310.94674005448</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="O35">
+        <f>AVERAGE(O31:O33)</f>
+        <v>4.6565606524115966</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>0</v>
+      </c>
+      <c r="B38">
+        <v>40</v>
+      </c>
+      <c r="C38">
+        <v>0.10166666670000001</v>
+      </c>
+      <c r="D38">
+        <v>0.15333333330000001</v>
+      </c>
+      <c r="E38">
+        <v>0.19500000000000001</v>
+      </c>
+      <c r="F38">
+        <v>0.2416666667</v>
+      </c>
+      <c r="G38">
+        <v>0.30166666669999997</v>
+      </c>
+      <c r="H38">
+        <v>0.34</v>
+      </c>
+      <c r="I38">
+        <v>0.37666666669999999</v>
+      </c>
+      <c r="J38">
+        <v>0.41666666670000002</v>
+      </c>
+      <c r="K38">
+        <v>0.46666666670000001</v>
+      </c>
+      <c r="N38">
+        <f>INTERCEPT($C$29:$K$29,C38:K38)</f>
+        <v>-8.9681311696553356E-2</v>
+      </c>
+      <c r="O38">
+        <f>SLOPE($C$29:$K$29,C38:K38)</f>
+        <v>5.516888870571786</v>
+      </c>
+      <c r="P38" s="3">
+        <f>O38*$P$24*$Q$24</f>
+        <v>0.34795720373548145</v>
+      </c>
+      <c r="Q38">
+        <v>25.9</v>
+      </c>
+      <c r="R38">
+        <f>(Q38/$R$24)*1000</f>
+        <v>178574.26034748208</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B39">
+        <v>40</v>
+      </c>
+      <c r="C39">
+        <v>6.8333333329999996E-2</v>
+      </c>
+      <c r="D39">
+        <v>0.1333333333</v>
+      </c>
+      <c r="E39">
+        <v>0.18166666670000001</v>
+      </c>
+      <c r="F39">
+        <v>0.24</v>
+      </c>
+      <c r="G39">
+        <v>0.28166666670000001</v>
+      </c>
+      <c r="H39">
+        <v>0.32333333330000003</v>
+      </c>
+      <c r="I39">
+        <v>0.36666666669999998</v>
+      </c>
+      <c r="J39">
+        <v>0.41333333329999999</v>
+      </c>
+      <c r="K39">
+        <v>0.45500000000000002</v>
+      </c>
+      <c r="N39">
+        <f>INTERCEPT($C$29:$K$29,C39:K39)</f>
+        <v>6.0745014490740434E-2</v>
+      </c>
+      <c r="O39">
+        <f>SLOPE($C$29:$K$29,C39:K39)</f>
+        <v>5.2584417603251126</v>
+      </c>
+      <c r="P39" s="3">
+        <f>O39*$P$24*$Q$24</f>
+        <v>0.33165661550455922</v>
+      </c>
+      <c r="Q39">
+        <v>23.9</v>
+      </c>
+      <c r="R39">
+        <f>(Q39/$R$24)*1000</f>
+        <v>164784.74217393133</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B40">
+        <v>40</v>
+      </c>
+      <c r="C40">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="D40">
+        <v>0.1416666667</v>
+      </c>
+      <c r="E40">
+        <v>0.1983333333</v>
+      </c>
+      <c r="F40">
+        <v>0.255</v>
+      </c>
+      <c r="G40">
+        <v>0.30666666669999998</v>
+      </c>
+      <c r="H40">
+        <v>0.3533333333</v>
+      </c>
+      <c r="I40">
+        <v>0.40333333329999999</v>
+      </c>
+      <c r="J40">
+        <v>0.46500000000000002</v>
+      </c>
+      <c r="K40">
+        <v>0.50166666670000004</v>
+      </c>
+      <c r="N40">
+        <f>INTERCEPT($C$29:$K$29,C40:K40)</f>
+        <v>4.1699761712626016E-2</v>
+      </c>
+      <c r="O40">
+        <f>SLOPE($C$29:$K$29,C40:K40)</f>
+        <v>4.8252581413920472</v>
+      </c>
+      <c r="P40" s="3">
+        <f>O40*$P$24*$Q$24</f>
+        <v>0.3043351732416949</v>
+      </c>
+      <c r="Q40">
+        <v>16.2</v>
+      </c>
+      <c r="R40">
+        <f>(Q40/$R$24)*1000</f>
+        <v>111695.09720576099</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>1</v>
+      </c>
+      <c r="C42">
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="D42">
+        <v>0.245</v>
+      </c>
+      <c r="E42">
+        <v>0.31833333330000002</v>
+      </c>
+      <c r="F42">
+        <v>0.40166666670000001</v>
+      </c>
+      <c r="G42">
+        <v>0.4833333333</v>
+      </c>
+      <c r="H42">
+        <v>0.57499999999999996</v>
+      </c>
+      <c r="I42">
+        <v>0.63166666670000005</v>
+      </c>
+      <c r="J42">
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="K42">
+        <v>0.77333333329999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>